<commit_message>
omitted the important information
</commit_message>
<xml_diff>
--- a/supports/questions.xlsx
+++ b/supports/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shry398828336/signpost-test/supports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C832CCD-8895-0D44-A98C-19A23FAD65D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FD39A9-EA3B-7A45-A626-D0B0E8951F79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="980" windowWidth="16040" windowHeight="15860" xr2:uid="{C1EA4480-BE33-CF4B-8634-E614821F8287}"/>
+    <workbookView xWindow="760" yWindow="980" windowWidth="27660" windowHeight="15860" xr2:uid="{C1EA4480-BE33-CF4B-8634-E614821F8287}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="216">
   <si>
     <t>At a party, do you:</t>
   </si>
@@ -315,147 +315,9 @@
     <t>“Speak for themselves”.</t>
   </si>
   <si>
-    <t>somewhat annoying.</t>
-  </si>
-  <si>
-    <t>a cool-headed person.</t>
-  </si>
-  <si>
-    <t>unjust.</t>
-  </si>
-  <si>
-    <t>by careful selection and choice.</t>
-  </si>
-  <si>
-    <t>having purchased.</t>
-  </si>
-  <si>
-    <t>initiate conversation.</t>
-  </si>
-  <si>
-    <t>rarely questionable.</t>
-  </si>
-  <si>
-    <t>make themselves useful enough.</t>
-  </si>
-  <si>
-    <t>standards.</t>
-  </si>
-  <si>
-    <t>firm than gentle.</t>
-  </si>
-  <si>
-    <t>the ability to organize and be methodical.</t>
-  </si>
-  <si>
-    <t>infinite.</t>
-  </si>
-  <si>
-    <t>stimulate and energize you.</t>
-  </si>
-  <si>
-    <t>a practical sort of person.</t>
-  </si>
-  <si>
-    <t>see how others are useful.</t>
-  </si>
-  <si>
-    <t>to discuss an issue thoroughly.</t>
-  </si>
-  <si>
-    <t>your head.</t>
-  </si>
-  <si>
-    <t>contracted.</t>
-  </si>
-  <si>
-    <t>the orderly.</t>
-  </si>
-  <si>
-    <t>many friends with brief contact.</t>
-  </si>
-  <si>
-    <t>facts.</t>
-  </si>
-  <si>
-    <t>production and distribution.</t>
-  </si>
-  <si>
     <t>“There is a very logical person.”.</t>
   </si>
   <si>
-    <t>unwavering.</t>
-  </si>
-  <si>
-    <t>final and unalterable statement.</t>
-  </si>
-  <si>
-    <t>after a decision.</t>
-  </si>
-  <si>
-    <t>speak easily and at length with strangers.</t>
-  </si>
-  <si>
-    <t>experience.</t>
-  </si>
-  <si>
-    <t>more practical than ingenious.</t>
-  </si>
-  <si>
-    <t>clear reason.</t>
-  </si>
-  <si>
-    <t>fair-minded.</t>
-  </si>
-  <si>
-    <t>make sure things are arranged.</t>
-  </si>
-  <si>
-    <t>re-negotiable.</t>
-  </si>
-  <si>
-    <t>hasten to get to it first.</t>
-  </si>
-  <si>
-    <t>a strong sense of reality.</t>
-  </si>
-  <si>
-    <t>fundamentals.</t>
-  </si>
-  <si>
-    <t>to be too passionate.</t>
-  </si>
-  <si>
-    <t>hard-headed.</t>
-  </si>
-  <si>
-    <t>the structured and scheduled.</t>
-  </si>
-  <si>
-    <t>routinized than whimsical.</t>
-  </si>
-  <si>
-    <t>easy to approach.</t>
-  </si>
-  <si>
-    <t>the more literal.</t>
-  </si>
-  <si>
-    <t>identify with others.</t>
-  </si>
-  <si>
-    <t>clarity of reason.</t>
-  </si>
-  <si>
-    <t>being indiscriminate.</t>
-  </si>
-  <si>
-    <t>planned event.</t>
-  </si>
-  <si>
-    <t>deliberate than spontaneous.</t>
-  </si>
-  <si>
     <t>Be “in a rut”.</t>
   </si>
   <si>
@@ -519,147 +381,9 @@
     <t>Illustrate principles.</t>
   </si>
   <si>
-    <t>rather fascinating.</t>
-  </si>
-  <si>
-    <t>a warm-hearted person.</t>
-  </si>
-  <si>
-    <t>merciless.</t>
-  </si>
-  <si>
-    <t>randomly and by chance.</t>
-  </si>
-  <si>
-    <t>having the option to buy.</t>
-  </si>
-  <si>
-    <t>wait to be approached.</t>
-  </si>
-  <si>
-    <t>frequently questionable.</t>
-  </si>
-  <si>
-    <t>exercise their fantasy enough.</t>
-  </si>
-  <si>
-    <t>feelings.</t>
-  </si>
-  <si>
-    <t>gentle than firm.</t>
-  </si>
-  <si>
-    <t>the ability to adapt and make do.</t>
-  </si>
-  <si>
-    <t>open-minded.</t>
-  </si>
-  <si>
-    <t>tax your reserves.</t>
-  </si>
-  <si>
-    <t>a fanciful sort of person.</t>
-  </si>
-  <si>
-    <t>see how others see.</t>
-  </si>
-  <si>
-    <t>to arrive at agreement on an issue.</t>
-  </si>
-  <si>
-    <t>your heart.</t>
-  </si>
-  <si>
-    <t>done on a casual basis.</t>
-  </si>
-  <si>
-    <t>whatever turns up.</t>
-  </si>
-  <si>
-    <t>a few friends with more lengthy contact.</t>
-  </si>
-  <si>
-    <t>principles.</t>
-  </si>
-  <si>
-    <t>design and research.</t>
-  </si>
-  <si>
     <t>“There is a very sentimental person.”.</t>
   </si>
   <si>
-    <t>devoted.</t>
-  </si>
-  <si>
-    <t>tentative and preliminary statement.</t>
-  </si>
-  <si>
-    <t>before a decision.</t>
-  </si>
-  <si>
-    <t>find little to say to strangers.</t>
-  </si>
-  <si>
-    <t>hunch.</t>
-  </si>
-  <si>
-    <t>more ingenious than practical.</t>
-  </si>
-  <si>
-    <t>strong feeling.</t>
-  </si>
-  <si>
-    <t>sympathetic.</t>
-  </si>
-  <si>
-    <t>just let things happen.</t>
-  </si>
-  <si>
-    <t>random and circumstantial.</t>
-  </si>
-  <si>
-    <t>hope someone else will answer.</t>
-  </si>
-  <si>
-    <t>a vivid imagination.</t>
-  </si>
-  <si>
-    <t>overtones.</t>
-  </si>
-  <si>
-    <t>to be too objective.</t>
-  </si>
-  <si>
-    <t>soft-hearted.</t>
-  </si>
-  <si>
-    <t>the unstructured and unscheduled.</t>
-  </si>
-  <si>
-    <t>whimsical than routinized.</t>
-  </si>
-  <si>
-    <t>somewhat reserved.</t>
-  </si>
-  <si>
-    <t>the more figurative.</t>
-  </si>
-  <si>
-    <t>utilize others.</t>
-  </si>
-  <si>
-    <t>strength of compassion.</t>
-  </si>
-  <si>
-    <t>being critical.</t>
-  </si>
-  <si>
-    <t>unplanned event.</t>
-  </si>
-  <si>
-    <t>spontaneous than deliberate.</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -685,13 +409,286 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>Somewhat annoying.</t>
+  </si>
+  <si>
+    <t>A cool-headed person.</t>
+  </si>
+  <si>
+    <t>Unjust.</t>
+  </si>
+  <si>
+    <t>By careful selection and choice.</t>
+  </si>
+  <si>
+    <t>Having purchased.</t>
+  </si>
+  <si>
+    <t>Initiate conversation.</t>
+  </si>
+  <si>
+    <t>Rarely questionable.</t>
+  </si>
+  <si>
+    <t>Make themselves useful enough.</t>
+  </si>
+  <si>
+    <t>Standards.</t>
+  </si>
+  <si>
+    <t>Firm than gentle.</t>
+  </si>
+  <si>
+    <t>The ability to organize and be methodical.</t>
+  </si>
+  <si>
+    <t>Infinite.</t>
+  </si>
+  <si>
+    <t>Stimulate and energize you.</t>
+  </si>
+  <si>
+    <t>A practical sort of person.</t>
+  </si>
+  <si>
+    <t>See how others are useful.</t>
+  </si>
+  <si>
+    <t>To discuss an issue thoroughly.</t>
+  </si>
+  <si>
+    <t>Your head.</t>
+  </si>
+  <si>
+    <t>Contracted.</t>
+  </si>
+  <si>
+    <t>The orderly.</t>
+  </si>
+  <si>
+    <t>Many friends with brief contact.</t>
+  </si>
+  <si>
+    <t>Facts.</t>
+  </si>
+  <si>
+    <t>Production and distribution.</t>
+  </si>
+  <si>
+    <t>Unwavering.</t>
+  </si>
+  <si>
+    <t>Final and unalterable statement.</t>
+  </si>
+  <si>
+    <t>After a decision.</t>
+  </si>
+  <si>
+    <t>Speak easily and at length with strangers.</t>
+  </si>
+  <si>
+    <t>Experience.</t>
+  </si>
+  <si>
+    <t>More practical than ingenious.</t>
+  </si>
+  <si>
+    <t>Clear reason.</t>
+  </si>
+  <si>
+    <t>Fair-minded.</t>
+  </si>
+  <si>
+    <t>Make sure things are arranged.</t>
+  </si>
+  <si>
+    <t>Re-negotiable.</t>
+  </si>
+  <si>
+    <t>Hasten to get to it first.</t>
+  </si>
+  <si>
+    <t>A strong sense of reality.</t>
+  </si>
+  <si>
+    <t>Fundamentals.</t>
+  </si>
+  <si>
+    <t>To be too passionate.</t>
+  </si>
+  <si>
+    <t>Hard-headed.</t>
+  </si>
+  <si>
+    <t>The structured and scheduled.</t>
+  </si>
+  <si>
+    <t>Routinized than whimsical.</t>
+  </si>
+  <si>
+    <t>Easy to approach.</t>
+  </si>
+  <si>
+    <t>The more literal.</t>
+  </si>
+  <si>
+    <t>Identify with others.</t>
+  </si>
+  <si>
+    <t>Clarity of reason.</t>
+  </si>
+  <si>
+    <t>Being indiscriminate.</t>
+  </si>
+  <si>
+    <t>Planned event.</t>
+  </si>
+  <si>
+    <t>Deliberate than spontaneous.</t>
+  </si>
+  <si>
+    <t>Rather fascinating.</t>
+  </si>
+  <si>
+    <t>A warm-hearted person.</t>
+  </si>
+  <si>
+    <t>Merciless.</t>
+  </si>
+  <si>
+    <t>Randomly and by chance.</t>
+  </si>
+  <si>
+    <t>Having the option to buy.</t>
+  </si>
+  <si>
+    <t>Wait to be approached.</t>
+  </si>
+  <si>
+    <t>Frequently questionable.</t>
+  </si>
+  <si>
+    <t>Exercise their fantasy enough.</t>
+  </si>
+  <si>
+    <t>Feelings.</t>
+  </si>
+  <si>
+    <t>Gentle than firm.</t>
+  </si>
+  <si>
+    <t>The ability to adapt and make do.</t>
+  </si>
+  <si>
+    <t>Open-minded.</t>
+  </si>
+  <si>
+    <t>Tax your reserves.</t>
+  </si>
+  <si>
+    <t>A fanciful sort of person.</t>
+  </si>
+  <si>
+    <t>See how others see.</t>
+  </si>
+  <si>
+    <t>To arrive at agreement on an issue.</t>
+  </si>
+  <si>
+    <t>Your heart.</t>
+  </si>
+  <si>
+    <t>Done on a casual basis.</t>
+  </si>
+  <si>
+    <t>Whatever turns up.</t>
+  </si>
+  <si>
+    <t>A few friends with more lengthy contact.</t>
+  </si>
+  <si>
+    <t>Design and research.</t>
+  </si>
+  <si>
+    <t>Devoted.</t>
+  </si>
+  <si>
+    <t>Tentative and preliminary statement.</t>
+  </si>
+  <si>
+    <t>Before a decision.</t>
+  </si>
+  <si>
+    <t>Find little to say to strangers.</t>
+  </si>
+  <si>
+    <t>Hunch.</t>
+  </si>
+  <si>
+    <t>More ingenious than practical.</t>
+  </si>
+  <si>
+    <t>Strong feeling.</t>
+  </si>
+  <si>
+    <t>Sympathetic.</t>
+  </si>
+  <si>
+    <t>Just let things happen.</t>
+  </si>
+  <si>
+    <t>Random and circumstantial.</t>
+  </si>
+  <si>
+    <t>Hope someone else will answer.</t>
+  </si>
+  <si>
+    <t>A vivid imagination.</t>
+  </si>
+  <si>
+    <t>Overtones.</t>
+  </si>
+  <si>
+    <t>To be too objective.</t>
+  </si>
+  <si>
+    <t>Soft-hearted.</t>
+  </si>
+  <si>
+    <t>The unstructured and unscheduled.</t>
+  </si>
+  <si>
+    <t>Whimsical than routinized.</t>
+  </si>
+  <si>
+    <t>Somewhat reserved.</t>
+  </si>
+  <si>
+    <t>The more figurative.</t>
+  </si>
+  <si>
+    <t>Utilize others.</t>
+  </si>
+  <si>
+    <t>Strength of compassion.</t>
+  </si>
+  <si>
+    <t>Being critical.</t>
+  </si>
+  <si>
+    <t>Unplanned event.</t>
+  </si>
+  <si>
+    <t>Spontaneous than deliberate.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -704,6 +701,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF333333"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -726,9 +730,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1043,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC37660F-085B-B147-A058-44EBF0F36830}">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1054,7 +1059,7 @@
     <col min="1" max="6" width="41" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1062,22 +1067,23 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>208</v>
+        <v>116</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1085,22 +1091,23 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1108,22 +1115,23 @@
         <v>72</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1131,22 +1139,23 @@
         <v>73</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1154,22 +1163,23 @@
         <v>74</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1177,22 +1187,23 @@
         <v>75</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1200,22 +1211,23 @@
         <v>76</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1223,22 +1235,23 @@
         <v>77</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>208</v>
+        <v>116</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1246,22 +1259,23 @@
         <v>78</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>146</v>
+        <v>100</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1269,22 +1283,23 @@
         <v>79</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1292,22 +1307,23 @@
         <v>80</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1315,22 +1331,23 @@
         <v>81</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>149</v>
+        <v>103</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1338,22 +1355,23 @@
         <v>82</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -1361,22 +1379,23 @@
         <v>83</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1384,22 +1403,23 @@
         <v>84</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>208</v>
+        <v>116</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -1407,22 +1427,23 @@
         <v>85</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1430,22 +1451,23 @@
         <v>86</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -1453,22 +1475,23 @@
         <v>87</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>155</v>
+        <v>109</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -1476,22 +1499,23 @@
         <v>88</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -1499,22 +1523,23 @@
         <v>89</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -1522,22 +1547,23 @@
         <v>90</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1545,22 +1571,23 @@
         <v>91</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>208</v>
+        <v>116</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -1568,1101 +1595,1149 @@
         <v>92</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>208</v>
+        <v>116</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>208</v>
+        <v>116</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>208</v>
+        <v>116</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>181</v>
+        <v>73</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="G46" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>208</v>
+        <v>116</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>208</v>
+        <v>116</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>208</v>
+        <v>116</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>135</v>
+        <v>166</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>209</v>
+        <v>117</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>136</v>
+        <v>167</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>137</v>
+        <v>168</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>210</v>
+        <v>118</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>139</v>
+        <v>170</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>215</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="H70" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add new features: 1. Added a loading signing on buttons that needs to query the database; 2. Added a hovering style on navigator items. 3. Added an access of login interface. 4. Re-make the test-lists logic. 5. Enhanced the search function. Searching in description and upper or lower letters don't matter any more. 6. Highlighted the search terms.         Fixed bugs: 1. Overload on successively clicking random test button. 2. All logo area now is clickable.
</commit_message>
<xml_diff>
--- a/supports/questions.xlsx
+++ b/supports/questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shry398828336/signpost-test/supports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FD39A9-EA3B-7A45-A626-D0B0E8951F79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC320D6-670D-B540-9867-78B3421145C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="980" windowWidth="27660" windowHeight="15860" xr2:uid="{C1EA4480-BE33-CF4B-8634-E614821F8287}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>Interact with many, include strangers.</t>
   </si>
   <si>
-    <t>Bewteen A and B.</t>
-  </si>
-  <si>
     <t>Interact with a few, known to you.</t>
   </si>
   <si>
@@ -682,6 +679,9 @@
   </si>
   <si>
     <t>Spontaneous than deliberate.</t>
+  </si>
+  <si>
+    <t>Between A and B.</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1051,7 @@
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1067,1675 +1067,1675 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H52" s="2"/>
     </row>
     <row r="53" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H54" s="2"/>
     </row>
     <row r="55" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H56" s="2"/>
     </row>
     <row r="57" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H58" s="2"/>
     </row>
     <row r="59" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H59" s="2"/>
     </row>
     <row r="60" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H60" s="2"/>
     </row>
     <row r="61" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H61" s="2"/>
     </row>
     <row r="62" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H62" s="2"/>
     </row>
     <row r="63" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H63" s="2"/>
     </row>
     <row r="64" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H64" s="2"/>
     </row>
     <row r="65" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H65" s="2"/>
     </row>
     <row r="66" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H66" s="2"/>
     </row>
     <row r="67" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H67" s="2"/>
     </row>
     <row r="68" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H68" s="2"/>
     </row>
     <row r="69" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H69" s="2"/>
     </row>
     <row r="70" spans="1:8" ht="23" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H70" s="2"/>
     </row>

</xml_diff>